<commit_message>
[DSD-2063] merging develop to 1.2.0.1 (#221)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ABF47C-ED22-434A-9978-DA641204EF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6812" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="648">
   <si>
     <t>lang_code</t>
   </si>
@@ -1822,13 +1821,163 @@
   </si>
   <si>
     <t>vid-card-download-negative-purpose</t>
+  </si>
+  <si>
+    <t>mosip.idp.otp.template.property</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>mosip.idp.biometrics.template.property</t>
+  </si>
+  <si>
+    <t>Biometrics</t>
+  </si>
+  <si>
+    <t>mosip.idp.unknown.authentication.template.property</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>mosip.full.name.template.property</t>
+  </si>
+  <si>
+    <t>mosip.date.of.birth.template.property</t>
+  </si>
+  <si>
+    <t>mosip.uin.template.property</t>
+  </si>
+  <si>
+    <t>mosip.perpetual.vid.template.property</t>
+  </si>
+  <si>
+    <t>mosip.phone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.email.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.template.property</t>
+  </si>
+  <si>
+    <t>mosip.gender.template.property</t>
+  </si>
+  <si>
+    <t>mosip.defualt.template.property</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>UIN</t>
+  </si>
+  <si>
+    <t>Perpetual VID</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Defualt</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>vid-card-type</t>
+  </si>
+  <si>
+    <t>Vid Card Type</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>Request received email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-subject</t>
+  </si>
+  <si>
+    <t>Success email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-subject</t>
+  </si>
+  <si>
+    <t>Failure email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-content</t>
+  </si>
+  <si>
+    <t>Request received email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-content</t>
+  </si>
+  <si>
+    <t>Success email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-content</t>
+  </si>
+  <si>
+    <t>Failure email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received_SMS</t>
+  </si>
+  <si>
+    <t>Request received sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success_SMS</t>
+  </si>
+  <si>
+    <t>Success sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure_SMS</t>
+  </si>
+  <si>
+    <t>Failure sms to download my VID card</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_SMS</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject SMS</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1851,6 +2000,12 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -1890,7 +2045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1901,6 +2056,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1932,7 +2090,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2210,18 +2368,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1703"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1688" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1703" sqref="B1703"/>
+    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1730" sqref="F1730"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -26066,8 +26224,568 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1704" spans="1:4">
+      <c r="A1704" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1704" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>599</v>
+      </c>
+      <c r="D1704" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:4">
+      <c r="A1705" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1705" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>601</v>
+      </c>
+      <c r="D1705" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:4">
+      <c r="A1706" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1706" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>603</v>
+      </c>
+      <c r="D1706" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:4">
+      <c r="A1707" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>613</v>
+      </c>
+      <c r="D1707" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:4">
+      <c r="A1708" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>605</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1708" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:4">
+      <c r="A1709" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1709" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:4">
+      <c r="A1710" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1710" t="s">
+        <v>616</v>
+      </c>
+      <c r="D1710" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:4">
+      <c r="A1711" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1711" t="s">
+        <v>617</v>
+      </c>
+      <c r="D1711" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:4">
+      <c r="A1712" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1712" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1712" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:4">
+      <c r="A1713" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>610</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>618</v>
+      </c>
+      <c r="D1713" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:4">
+      <c r="A1714" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1714" t="s">
+        <v>619</v>
+      </c>
+      <c r="D1714" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:4">
+      <c r="A1715" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1715" t="s">
+        <v>620</v>
+      </c>
+      <c r="D1715" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:4">
+      <c r="A1716" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1716" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:4">
+      <c r="A1717" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1717" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:4">
+      <c r="A1718" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1718" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:4">
+      <c r="A1719" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>628</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1719" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:4">
+      <c r="A1720" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>630</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1720" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:4">
+      <c r="A1721" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>632</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>633</v>
+      </c>
+      <c r="D1721" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:4">
+      <c r="A1722" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>634</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>635</v>
+      </c>
+      <c r="D1722" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:4">
+      <c r="A1723" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>636</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>637</v>
+      </c>
+      <c r="D1723" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:4">
+      <c r="A1724" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>638</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>639</v>
+      </c>
+      <c r="D1724" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:4">
+      <c r="A1725" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>640</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>641</v>
+      </c>
+      <c r="D1725" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:4">
+      <c r="A1726" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1726" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:4">
+      <c r="A1727" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1727" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:4">
+      <c r="A1728" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1728" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4">
+      <c r="A1729" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1729" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4">
+      <c r="A1730" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1730" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4">
+      <c r="A1731" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1731" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4">
+      <c r="A1732" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1732" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4">
+      <c r="A1733" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1733" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4">
+      <c r="A1734" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1734" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:4">
+      <c r="A1735" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1735" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:4">
+      <c r="A1736" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1736" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:4">
+      <c r="A1737" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1737" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:4">
+      <c r="A1738" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1738" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:4">
+      <c r="A1739" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1739" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:4">
+      <c r="A1740" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1740" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:4">
+      <c r="A1741" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1741" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:4">
+      <c r="A1742" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1742" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:4">
+      <c r="A1743" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1743" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D400"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
DSD-3609 Removed duplicate code for template type code RPR_SUP_REJECT (#267)
* Move develop template.xlsx and template_type.xlsx
to 1.2.0.1

* DSD-3609 Added location for spa language.

* DSD-3609 Removed duplicate code for template type code RPR_SUP_REJECT_EMAIL_SUBJECT.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A72B4D-BA1A-4992-9B77-3DB127B7494C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D67A2A-6DCA-4473-9B8D-71040041915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1773</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1767</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7092" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7068" uniqueCount="684">
   <si>
     <t>lang_code</t>
   </si>
@@ -2478,17 +2478,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1773"/>
+  <dimension ref="A1:D1767"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A1753" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1762" sqref="E1762"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="37.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.54296875" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="1"/>
+    <col min="4" max="4" width="8.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -27150,10 +27150,10 @@
         <v>4</v>
       </c>
       <c r="B1762" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1762" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1762" s="1" t="s">
         <v>7</v>
@@ -27164,10 +27164,10 @@
         <v>293</v>
       </c>
       <c r="B1763" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1763" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1763" s="1" t="s">
         <v>7</v>
@@ -27178,10 +27178,10 @@
         <v>294</v>
       </c>
       <c r="B1764" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1764" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1764" s="1" t="s">
         <v>7</v>
@@ -27192,10 +27192,10 @@
         <v>302</v>
       </c>
       <c r="B1765" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1765" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1765" s="1" t="s">
         <v>7</v>
@@ -27206,10 +27206,10 @@
         <v>301</v>
       </c>
       <c r="B1766" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1766" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1766" s="1" t="s">
         <v>7</v>
@@ -27220,101 +27220,17 @@
         <v>303</v>
       </c>
       <c r="B1767" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1767" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1767" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="1768" spans="1:4">
-      <c r="A1768" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1768" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1768" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1768" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1769" spans="1:4">
-      <c r="A1769" t="s">
-        <v>293</v>
-      </c>
-      <c r="B1769" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1769" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1769" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1770" spans="1:4">
-      <c r="A1770" t="s">
-        <v>294</v>
-      </c>
-      <c r="B1770" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1770" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1770" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1771" spans="1:4">
-      <c r="A1771" t="s">
-        <v>302</v>
-      </c>
-      <c r="B1771" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1771" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1771" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1772" spans="1:4">
-      <c r="A1772" t="s">
-        <v>301</v>
-      </c>
-      <c r="B1772" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1772" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1772" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1773" spans="1:4">
-      <c r="A1773" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1773" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1773" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1773" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D1773" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D1767" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
DSD-3609 Removed duplicate code for template type code RPR_SUP_REJECT_EMAIL_SUBJECT. (#268)
* Move develop template.xlsx and template_type.xlsx
to 1.2.0.1

* DSD-3609 Added location for spa language.

* DSD-3609 Removed duplicate code for template type code RPR_SUP_REJECT_EMAIL_SUBJECT.

* DSD-3609 Removed duplicate code for template type code RPR_SUP_REJECT_EMAIL_SUBJECT.

* DSD-3609 Removed duplicate code for template type code
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D67A2A-6DCA-4473-9B8D-71040041915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10A25E7-F483-4FEC-9FF5-FDD52262045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1767</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1761</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7068" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="684">
   <si>
     <t>lang_code</t>
   </si>
@@ -2478,10 +2478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1767"/>
+  <dimension ref="A1:D1761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1753" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1762" sqref="E1762"/>
+    <sheetView tabSelected="1" topLeftCell="A1743" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1750" sqref="B1750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -27145,92 +27145,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1762" spans="1:4">
-      <c r="A1762" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1762" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1762" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1762" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1763" spans="1:4">
-      <c r="A1763" t="s">
-        <v>293</v>
-      </c>
-      <c r="B1763" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1763" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1763" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1764" spans="1:4">
-      <c r="A1764" t="s">
-        <v>294</v>
-      </c>
-      <c r="B1764" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1764" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1764" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1765" spans="1:4">
-      <c r="A1765" t="s">
-        <v>302</v>
-      </c>
-      <c r="B1765" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1765" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1765" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1766" spans="1:4">
-      <c r="A1766" t="s">
-        <v>301</v>
-      </c>
-      <c r="B1766" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1766" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1766" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1767" spans="1:4">
-      <c r="A1767" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1767" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1767" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1767" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D1767" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D1761" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated template and template_type to remove duplicate template type code. (#271)
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10A25E7-F483-4FEC-9FF5-FDD52262045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FCA463-3D86-4AC6-9C36-CA205CF91E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7048" uniqueCount="686">
   <si>
     <t>lang_code</t>
   </si>
@@ -2080,13 +2080,19 @@
   </si>
   <si>
     <t>Locked status</t>
+  </si>
+  <si>
+    <t>reg-consent-template</t>
+  </si>
+  <si>
+    <t>Registration Client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2117,6 +2123,12 @@
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2154,7 +2166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2170,6 +2182,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2478,10 +2491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1761"/>
+  <dimension ref="A1:D1762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1743" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1750" sqref="B1750"/>
+    <sheetView tabSelected="1" topLeftCell="A1758" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1763" sqref="C1763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -27145,6 +27158,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1762" spans="1:4">
+      <c r="A1762" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1762" t="s">
+        <v>684</v>
+      </c>
+      <c r="C1762" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="D1762" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1761" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-32404 Added develop templates to release 121x
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5EB0D0-87C3-4CE9-93D3-92F00E415A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F43346-CCEB-4C34-BCBD-E7555BAEFE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9192" uniqueCount="1399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9240" uniqueCount="1400">
   <si>
     <t>lang_code</t>
   </si>
@@ -5719,6 +5719,9 @@
   </si>
   <si>
     <t>Regproc success summary to self update demographic data</t>
+  </si>
+  <si>
+    <t>spa</t>
   </si>
 </sst>
 </file>
@@ -6186,10 +6189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2298"/>
+  <dimension ref="A1:D2310"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2294" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2310" sqref="E2310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -38360,15 +38363,183 @@
     </row>
     <row r="2298" spans="1:4">
       <c r="A2298" t="s">
-        <v>4</v>
+        <v>1399</v>
       </c>
       <c r="B2298" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C2298" s="8" t="s">
         <v>1398</v>
       </c>
       <c r="D2298" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:4">
+      <c r="A2299" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2299" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C2299" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2299" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:4">
+      <c r="A2300" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2300" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C2300" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2300" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:4">
+      <c r="A2301" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2301" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C2301" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2301" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:4">
+      <c r="A2302" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2302" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C2302" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2302" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:4">
+      <c r="A2303" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2303" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C2303" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2303" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:4">
+      <c r="A2304" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2304" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2304" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2304" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:4">
+      <c r="A2305" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B2305" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2305" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2305" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:4">
+      <c r="A2306" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2306" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2306" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2306" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:4">
+      <c r="A2307" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2307" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2307" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2307" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:4">
+      <c r="A2308" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2308" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2308" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2308" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:4">
+      <c r="A2309" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2309" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2309" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2309" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:4">
+      <c r="A2310" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2310" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2310" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2310" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>